<commit_message>
Added documentation and example for the questionnaire
</commit_message>
<xml_diff>
--- a/docs/data/simple-questionnaire.xlsx
+++ b/docs/data/simple-questionnaire.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-32240" yWindow="-180" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-38620" yWindow="-740" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="1" r:id="rId1"/>
@@ -79,18 +79,6 @@
     <t>Hidden ID used as a unique key for every questionnaire row</t>
   </si>
   <si>
-    <t>birthdate</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>Date of birth</t>
-  </si>
-  <si>
-    <t>What is your date of birth?</t>
-  </si>
-  <si>
     <t>driverslicence</t>
   </si>
   <si>
@@ -103,7 +91,19 @@
     <t>Drivers license</t>
   </si>
   <si>
-    <t>$('birthdate').age().ge(18).value()</t>
+    <t>age</t>
+  </si>
+  <si>
+    <t>$('age').ge(18).value()</t>
+  </si>
+  <si>
+    <t>What is your age?</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Age</t>
   </si>
 </sst>
 </file>
@@ -213,8 +213,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -229,13 +235,19 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -568,7 +580,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -609,7 +621,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -623,7 +634,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -695,16 +706,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -712,24 +723,23 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
doc: replace magma references in docs
</commit_message>
<xml_diff>
--- a/docs/data/simple-questionnaire.xlsx
+++ b/docs/data/simple-questionnaire.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkelpin/git/molgenis/docs/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62EC311-3CA4-6C44-A14E-1441299B9965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38620" yWindow="-740" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="1" r:id="rId1"/>
     <sheet name="attributes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -94,9 +100,6 @@
     <t>age</t>
   </si>
   <si>
-    <t>$('age').ge(18).value()</t>
-  </si>
-  <si>
     <t>What is your age?</t>
   </si>
   <si>
@@ -104,12 +107,15 @@
   </si>
   <si>
     <t>Age</t>
+  </si>
+  <si>
+    <t>{age} &gt;= 18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -252,6 +258,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -576,14 +590,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
@@ -591,7 +605,7 @@
     <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -605,7 +619,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -630,14 +644,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
@@ -646,7 +660,7 @@
     <col min="9" max="9" width="49.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
+    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -675,7 +689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -701,7 +715,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -709,16 +723,16 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>27</v>
-      </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -729,7 +743,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
doc: fix sample questionnaire
Fixes #9248
</commit_message>
<xml_diff>
--- a/docs/data/simple-questionnaire.xlsx
+++ b/docs/data/simple-questionnaire.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkelpin/git/molgenis/docs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62EC311-3CA4-6C44-A14E-1441299B9965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571D179D-DD1D-C244-AA29-DAFFBCC04648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33620" yWindow="-11840" windowWidth="28800" windowHeight="16320" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="entities" sheetId="1" r:id="rId1"/>
-    <sheet name="attributes" sheetId="2" r:id="rId2"/>
+    <sheet name="packages" sheetId="3" r:id="rId1"/>
+    <sheet name="entities" sheetId="1" r:id="rId2"/>
+    <sheet name="attributes" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>name</t>
   </si>
@@ -91,9 +92,6 @@
     <t>bool</t>
   </si>
   <si>
-    <t>Do you have a drivers license</t>
-  </si>
-  <si>
     <t>Drivers license</t>
   </si>
   <si>
@@ -110,6 +108,33 @@
   </si>
   <si>
     <t>{age} &gt;= 18</t>
+  </si>
+  <si>
+    <t>labelAttribute</t>
+  </si>
+  <si>
+    <t>doc</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Sample data</t>
+  </si>
+  <si>
+    <t>package</t>
+  </si>
+  <si>
+    <t>doc_SimpleQuestionnaire</t>
+  </si>
+  <si>
+    <t>What is your name?</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Do you have a drivers license?</t>
   </si>
 </sst>
 </file>
@@ -590,46 +615,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6E84D6-0973-4146-A2EC-DA3B54E30A64}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="D1" sqref="D1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -643,24 +717,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="49.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -677,21 +753,24 @@
         <v>12</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -702,54 +781,77 @@
       <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
       <c r="G2" t="b">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="b">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="J4" t="s">
         <v>25</v>
       </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
         <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>